<commit_message>
added some questionaire results and updated the report
</commit_message>
<xml_diff>
--- a/Materials/Requirements/Functional Requirements.xlsx
+++ b/Materials/Requirements/Functional Requirements.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27815"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilrafferty/Downloads/COM562 - Computing Project/workspace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neilrafferty/Downloads/COM562 - Computing Project/workspace/Materials/Requirements/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="38320" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Functional Requirement Table" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="931" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="390">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -306,9 +306,6 @@
     <t>Step 1: The user should select the log out button</t>
   </si>
   <si>
-    <t>The user will be able to sever the connection to there account.</t>
-  </si>
-  <si>
     <t>This will allow the user to unauthenticated themselves encase they are on a shared machine or if they want to log in as another user.</t>
   </si>
   <si>
@@ -690,9 +687,6 @@
     <t>Step 6: The UI will be refreshed.</t>
   </si>
   <si>
-    <t>A user will be able to flag a contact for several different reasons.</t>
-  </si>
-  <si>
     <t>This will help users make more informed decisions.</t>
   </si>
   <si>
@@ -1191,12 +1185,6 @@
     <t>The user should be able to edit a list of recovery contact information.</t>
   </si>
   <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>MVP</t>
-  </si>
-  <si>
     <t>User, Super User, Admin</t>
   </si>
   <si>
@@ -1213,6 +1201,30 @@
   </si>
   <si>
     <t>Step 2: Fill out and submit the registration form (this will consist of a password, unique username, and optional contact point for account recovery).</t>
+  </si>
+  <si>
+    <t>Messaging</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>Mail Rules</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>A user will be able to flag a contact for several different reasons for other users to see.</t>
+  </si>
+  <si>
+    <t>The user will be able to sever the connection to their account.</t>
   </si>
 </sst>
 </file>
@@ -1430,6 +1442,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1447,9 +1462,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -1742,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E240"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1751,8 +1763,8 @@
     <col min="1" max="1" width="18" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="28.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="4" max="4" width="16.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1766,10 +1778,10 @@
         <v>3</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>378</v>
+        <v>384</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1780,13 +1792,13 @@
         <v>5</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>379</v>
+        <v>371</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1797,13 +1809,13 @@
         <v>6</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1814,13 +1826,13 @@
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>379</v>
+        <v>371</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1831,13 +1843,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1845,16 +1857,16 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>379</v>
+        <v>371</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1865,13 +1877,13 @@
         <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1882,13 +1894,13 @@
         <v>15</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1899,13 +1911,13 @@
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1916,13 +1928,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1933,13 +1945,13 @@
         <v>17</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1947,16 +1959,16 @@
         <v>23</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1967,13 +1979,13 @@
         <v>19</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>379</v>
+        <v>385</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1981,30 +1993,34 @@
         <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E14" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E15" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
@@ -2014,12 +2030,14 @@
         <v>27</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E16" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
@@ -2029,12 +2047,14 @@
         <v>28</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E17" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
@@ -2044,27 +2064,31 @@
         <v>29</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E18" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
@@ -2074,12 +2098,14 @@
         <v>42</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E20" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
@@ -2089,12 +2115,14 @@
         <v>43</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E21" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
@@ -2104,57 +2132,65 @@
         <v>44</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E22" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E23" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>38</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C24" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E25" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
@@ -2164,12 +2200,14 @@
         <v>46</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E26" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
@@ -2179,27 +2217,31 @@
         <v>47</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>373</v>
-      </c>
-      <c r="E27" s="8"/>
+        <v>371</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>45</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C28" s="7" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>373</v>
-      </c>
-      <c r="E28" s="7"/>
+        <v>371</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>378</v>
+      </c>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
@@ -3286,7 +3328,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3316,7 +3358,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3324,7 +3366,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3332,7 +3374,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3340,7 +3382,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3348,7 +3390,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3356,7 +3398,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3364,7 +3406,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3372,43 +3414,43 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3416,7 +3458,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3467,7 +3509,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3475,7 +3517,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3483,7 +3525,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3499,7 +3541,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3507,7 +3549,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -3515,7 +3557,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3523,25 +3565,25 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3557,7 +3599,7 @@
         <v>61</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3584,7 +3626,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3600,7 +3642,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3608,7 +3650,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3616,7 +3658,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3632,7 +3674,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3640,7 +3682,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -3648,7 +3690,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3656,31 +3698,31 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3696,7 +3738,7 @@
         <v>61</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3709,7 +3751,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3739,7 +3781,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>211</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3747,7 +3789,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3755,7 +3797,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3763,7 +3805,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3771,7 +3813,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3779,7 +3821,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3787,7 +3829,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3795,37 +3837,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3868,7 +3910,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3884,7 +3926,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3892,7 +3934,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3900,7 +3942,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3916,7 +3958,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3924,7 +3966,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3932,7 +3974,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3940,37 +3982,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -3986,7 +4028,7 @@
         <v>61</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -4013,7 +4055,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4029,7 +4071,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4037,7 +4079,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4045,7 +4087,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4061,7 +4103,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4069,7 +4111,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4077,7 +4119,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4085,67 +4127,67 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="7" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="7" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4161,7 +4203,7 @@
         <v>61</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -4188,7 +4230,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4204,7 +4246,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4212,7 +4254,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4220,7 +4262,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4236,7 +4278,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4244,7 +4286,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4252,7 +4294,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4260,25 +4302,25 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4337,7 +4379,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4345,7 +4387,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4353,7 +4395,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4369,7 +4411,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4377,7 +4419,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4385,7 +4427,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4393,31 +4435,31 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="8" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4425,7 +4467,7 @@
         <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4476,7 +4518,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4484,7 +4526,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4492,7 +4534,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4508,7 +4550,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4516,7 +4558,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4524,7 +4566,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4532,43 +4574,43 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4576,7 +4618,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4611,7 +4653,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4627,7 +4669,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4635,7 +4677,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4643,7 +4685,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4659,7 +4701,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4667,7 +4709,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4675,7 +4717,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4683,43 +4725,43 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4727,7 +4769,7 @@
         <v>59</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4747,8 +4789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4786,7 +4828,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -4834,19 +4876,19 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="7" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="8" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -4858,7 +4900,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="18" t="s">
         <v>61</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -4905,7 +4947,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -4913,7 +4955,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C4" s="12"/>
     </row>
@@ -4922,7 +4964,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -4938,7 +4980,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -4946,7 +4988,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -4954,7 +4996,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -4962,37 +5004,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="8" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="8" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="8" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.2">
@@ -5051,7 +5093,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5059,7 +5101,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5067,7 +5109,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5083,7 +5125,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5091,7 +5133,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5099,7 +5141,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5107,37 +5149,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5196,7 +5238,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5204,7 +5246,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5212,7 +5254,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5228,7 +5270,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5236,7 +5278,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5244,7 +5286,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5252,37 +5294,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5325,7 +5367,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5341,7 +5383,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5349,7 +5391,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5357,7 +5399,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5365,7 +5407,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5373,7 +5415,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5381,7 +5423,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5389,7 +5431,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5397,19 +5439,19 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5417,7 +5459,7 @@
         <v>59</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5425,7 +5467,7 @@
         <v>61</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -5452,7 +5494,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5468,7 +5510,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5476,7 +5518,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5484,7 +5526,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5500,7 +5542,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5508,7 +5550,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5516,7 +5558,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5524,19 +5566,19 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5579,7 +5621,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5595,7 +5637,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5603,7 +5645,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5611,7 +5653,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5627,7 +5669,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5635,7 +5677,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5643,7 +5685,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5651,25 +5693,25 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5728,7 +5770,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5736,7 +5778,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5744,7 +5786,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5760,7 +5802,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5768,7 +5810,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5776,7 +5818,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5784,43 +5826,43 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="8" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="8" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="8" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5879,7 +5921,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5887,7 +5929,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5895,7 +5937,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5911,7 +5953,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -5919,7 +5961,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5927,7 +5969,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5935,37 +5977,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -5981,7 +6023,7 @@
         <v>61</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -6008,7 +6050,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6024,7 +6066,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6040,7 +6082,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6056,7 +6098,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6064,7 +6106,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6072,7 +6114,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6080,37 +6122,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6159,7 +6201,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6209,43 +6251,43 @@
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="9"/>
       <c r="B14" s="6" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="6" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6269,8 +6311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView zoomScale="92" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6308,7 +6350,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -6352,7 +6394,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -6360,13 +6402,13 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="21"/>
       <c r="B12" s="8" t="s">
         <v>76</v>
       </c>
@@ -6384,7 +6426,7 @@
         <v>61</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6409,7 +6451,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6439,7 +6481,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>83</v>
+        <v>389</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6447,7 +6489,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="33" customHeight="1" x14ac:dyDescent="0.2">
@@ -6455,7 +6497,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6491,7 +6533,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -6499,27 +6541,27 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="7" t="s">
+    <row r="14" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="21"/>
+      <c r="B14" s="8" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
-      <c r="B14" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -6527,7 +6569,7 @@
         <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -6551,7 +6593,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6581,7 +6623,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6589,7 +6631,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -6597,7 +6639,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6605,7 +6647,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6629,77 +6671,77 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>91</v>
-      </c>
-    </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
+      <c r="A11" s="20"/>
       <c r="B11" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="54" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
+      <c r="A12" s="20"/>
       <c r="B12" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="21"/>
       <c r="B13" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="19" t="s">
         <v>59</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="8" t="s">
-        <v>96</v>
-      </c>
-    </row>
     <row r="17" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
+      <c r="A17" s="20"/>
       <c r="B17" s="7" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="19"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A20" s="21"/>
+      <c r="B20" s="8" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A19" s="19"/>
-      <c r="B19" s="7" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="8" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -6707,7 +6749,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -6738,7 +6780,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6754,7 +6796,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6762,7 +6804,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6770,7 +6812,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6786,7 +6828,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6794,7 +6836,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6802,39 +6844,39 @@
         <v>57</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="23"/>
+      <c r="B11" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="23"/>
+      <c r="B12" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="22"/>
-      <c r="B12" s="6" t="s">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A13" s="23"/>
+      <c r="B13" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="5" t="s">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="6" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6850,7 +6892,7 @@
         <v>61</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -6865,8 +6907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="84" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView zoomScale="84" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6896,7 +6938,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6904,7 +6946,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6912,7 +6954,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6920,7 +6962,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6928,7 +6970,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -6936,7 +6978,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="36" x14ac:dyDescent="0.2">
@@ -6944,63 +6986,63 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="7" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="7" t="s">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="B12" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="B13" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="8" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="36" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="19"/>
-      <c r="B12" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A13" s="19"/>
-      <c r="B13" s="7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A14" s="19"/>
-      <c r="B14" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A15" s="19"/>
-      <c r="B15" s="7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A16" s="19"/>
-      <c r="B16" s="8" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A17" s="19"/>
-      <c r="B17" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="21"/>
       <c r="B18" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7012,17 +7054,17 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="36" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="19" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="21"/>
       <c r="B21" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -7039,7 +7081,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7053,7 +7095,7 @@
         <v>49</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7069,7 +7111,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7077,7 +7119,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7085,7 +7127,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7093,7 +7135,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7101,7 +7143,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7109,7 +7151,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7117,7 +7159,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7125,55 +7167,55 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7189,13 +7231,13 @@
         <v>61</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -7208,7 +7250,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7238,7 +7280,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7246,7 +7288,7 @@
         <v>52</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7254,7 +7296,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7262,7 +7304,7 @@
         <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7270,7 +7312,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7278,7 +7320,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7286,7 +7328,7 @@
         <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7294,37 +7336,37 @@
         <v>58</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
       <c r="B11" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
       <c r="B13" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
       <c r="B15" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7332,31 +7374,31 @@
         <v>59</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="36" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
       <c r="B19" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
       <c r="B20" s="8" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -7364,7 +7406,7 @@
         <v>61</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>